<commit_message>
Cập nhật kết nối online lên heroku
</commit_message>
<xml_diff>
--- a/public/schemas/Task.xlsx
+++ b/public/schemas/Task.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chức năng" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Cấu trúc chương trình" sheetId="4" r:id="rId3"/>
     <sheet name="Khai báo" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>STT</t>
   </si>
@@ -253,6 +253,18 @@
   </si>
   <si>
     <t>var [Tên biến route] = require([Path của route cần import])(app, pool);</t>
+  </si>
+  <si>
+    <t>b20a7ec83541b0</t>
+  </si>
+  <si>
+    <t>64ffe227</t>
+  </si>
+  <si>
+    <t>us-cdbr-iron-east-03.cleardb.net</t>
+  </si>
+  <si>
+    <t>heroku_633ee9287d27a78</t>
   </si>
 </sst>
 </file>
@@ -428,19 +440,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -495,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +570,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -966,6 +1006,9 @@
       <c r="B2" s="23" t="s">
         <v>35</v>
       </c>
+      <c r="C2" s="21" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -974,6 +1017,9 @@
       <c r="B3" s="23">
         <v>3306</v>
       </c>
+      <c r="C3" s="23">
+        <v>3306</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -982,6 +1028,9 @@
       <c r="B4" s="23" t="s">
         <v>37</v>
       </c>
+      <c r="C4" s="21" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
@@ -990,6 +1039,9 @@
       <c r="B5" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="C5" s="21" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
@@ -997,6 +1049,9 @@
       </c>
       <c r="B6" s="23" t="s">
         <v>39</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,29 +1075,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="27" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="26" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" style="20" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="29"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -1050,7 +1105,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -1058,7 +1113,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -1066,7 +1121,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -1074,7 +1129,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -1082,7 +1137,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -1090,22 +1145,22 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="29"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="20" t="s">
@@ -1113,7 +1168,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -1121,28 +1176,28 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1163,42 +1218,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>